<commit_message>
added validation examples to unit tests
Updated unit testing to consider the cases from validation section of documentation. Considered a less than 1% difference to commercial software "slide" to be an acceptable result.
</commit_message>
<xml_diff>
--- a/pyslope/examples/summary_results.xlsx
+++ b/pyslope/examples/summary_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesse\Dropbox\python\pySlope\PySlope\pyslope\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse\Desktop\pyslope\pyslope\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E66780-C70D-482A-9D75-CD775061AE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DE14D9-3DA3-401B-A54D-9FFBE526A1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{12948297-B713-4583-BCF4-D56AF65AEAD5}"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="28800" windowHeight="15210" activeTab="2" xr2:uid="{12948297-B713-4583-BCF4-D56AF65AEAD5}"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>pySlope</t>
   </si>
@@ -72,16 +72,27 @@
   </si>
   <si>
     <t>3.939</t>
+  </si>
+  <si>
+    <t>slide 500</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,10 +118,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -124,9 +136,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -438,15 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B435A3-EDD6-4F18-9DE5-7ACB0F97D5EF}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -460,7 +475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -473,8 +488,10 @@
       <c r="D2">
         <v>1.272</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -487,8 +504,10 @@
       <c r="D3">
         <v>2.1800000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -501,8 +520,10 @@
       <c r="D4">
         <v>3.907</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -515,6 +536,8 @@
       <c r="D5">
         <v>5.7359999999999998</v>
       </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -523,15 +546,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21E12E9-5D32-450C-A1F6-AABDC70C2A97}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="F1" sqref="F1:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -545,7 +568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -558,8 +581,10 @@
       <c r="D2">
         <v>1.272</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -572,8 +597,10 @@
       <c r="D3">
         <v>2.266</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -586,8 +613,10 @@
       <c r="D4">
         <v>3.9409999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -600,6 +629,8 @@
       <c r="D5">
         <v>5.7590000000000003</v>
       </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -608,15 +639,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D6C730-9398-424D-8EFB-1FE7695DCE91}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -629,8 +663,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -643,8 +680,13 @@
       <c r="D2">
         <v>1.607</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1.6020000000000001</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -657,8 +699,13 @@
       <c r="D3">
         <v>2.327</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2.33</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -671,6 +718,15 @@
       <c r="D4">
         <v>3.1960000000000002</v>
       </c>
+      <c r="E4" s="6">
+        <v>3.1739999999999999</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -679,15 +735,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817EC3CF-66E8-42DA-B5AC-B0979AC515C8}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -701,7 +757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -714,8 +770,10 @@
       <c r="D2">
         <v>1.597</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -728,8 +786,10 @@
       <c r="D3">
         <v>2.585</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -742,6 +802,8 @@
       <c r="D4">
         <v>4.266</v>
       </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -750,15 +812,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA947E7-32FB-4091-9A89-76664E0090EC}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -772,7 +834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -785,8 +847,10 @@
       <c r="D2">
         <v>2.036</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -799,8 +863,10 @@
       <c r="D3">
         <v>3.718</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -813,6 +879,8 @@
       <c r="D4">
         <v>5.5590000000000002</v>
       </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>